<commit_message>
Added paging for product list
</commit_message>
<xml_diff>
--- a/downloader/configuration.xlsx
+++ b/downloader/configuration.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$114</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="26">
   <si>
     <t>Nazev</t>
   </si>
@@ -37,6 +37,18 @@
     <t>Vedlejsi barvy</t>
   </si>
   <si>
+    <t>Hrneček malé kafíčko</t>
+  </si>
+  <si>
+    <t>muj typ</t>
+  </si>
+  <si>
+    <t>nejaky styl</t>
+  </si>
+  <si>
+    <t>a jeste barva</t>
+  </si>
+  <si>
     <t>Hrneček buclák</t>
   </si>
   <si>
@@ -50,6 +62,39 @@
   </si>
   <si>
     <t>Hrneček čtvrtlitrák</t>
+  </si>
+  <si>
+    <t>Hrnek půllitrák</t>
+  </si>
+  <si>
+    <t>Cukřenka</t>
+  </si>
+  <si>
+    <t>Džbán kónický</t>
+  </si>
+  <si>
+    <t>Zvonek Andělíček</t>
+  </si>
+  <si>
+    <t>Aromalampa</t>
+  </si>
+  <si>
+    <t>Hrneček presso</t>
+  </si>
+  <si>
+    <t>Hrneček piccolo</t>
+  </si>
+  <si>
+    <t>Talíř</t>
+  </si>
+  <si>
+    <t>Zvonek Andělka</t>
+  </si>
+  <si>
+    <t>Polévková miska</t>
+  </si>
+  <si>
+    <t>Aromalampa - květinový vzor</t>
   </si>
 </sst>
 </file>
@@ -113,7 +158,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="11979107_fzmzscbp-m.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="11979172_wrftiwzn-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -151,7 +196,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="11979104_cvzcurkk-m.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="11979168_qwzwgbzy-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -189,7 +234,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="11979097_syyocdql-m.jpg"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="11979165_kduptwic-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -227,7 +272,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="11979093_axmflveg-m.jpg"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="11979159_gmvayvld-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -265,7 +310,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="11979084_fjhfbrdu-m.jpg"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="11979157_awjoymip-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -303,7 +348,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="11979075_dpafjaua-m.jpg"/>
+        <xdr:cNvPr id="7" name="Picture 6" descr="11979153_tlfnoprn-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -341,7 +386,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="11979070_aogwrkdu-m.jpg"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="11979146_dbpxtnvf-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -379,7 +424,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="11979041_bvddbsaq-m.jpg"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="11979140_hadupqpg-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -417,7 +462,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="11979033_xbolvyqm-m.jpg"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="11979139_jjudsdry-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -455,7 +500,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="11979029_jxiajtun-m.jpg"/>
+        <xdr:cNvPr id="11" name="Picture 10" descr="11979129_ltmjrfkx-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -493,7 +538,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="11979023_nxxmpqll-m.jpg"/>
+        <xdr:cNvPr id="12" name="Picture 11" descr="11979107_fzmzscbp-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -531,7 +576,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="11979019_ppejxyhj-m.jpg"/>
+        <xdr:cNvPr id="13" name="Picture 12" descr="11979104_cvzcurkk-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -569,7 +614,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="11979016_bbckowbn-m.jpg"/>
+        <xdr:cNvPr id="14" name="Picture 13" descr="11979097_syyocdql-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -607,7 +652,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="11979010_bnwglwfx-m.jpg"/>
+        <xdr:cNvPr id="15" name="Picture 14" descr="11979093_axmflveg-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -645,7 +690,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="11979004_xitfbetj-m.jpg"/>
+        <xdr:cNvPr id="16" name="Picture 15" descr="11979084_fjhfbrdu-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -683,7 +728,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="11978901_vxrfzpph-m.jpg"/>
+        <xdr:cNvPr id="17" name="Picture 16" descr="11979075_dpafjaua-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -721,7 +766,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="11978900_yqmzthau-m.jpg"/>
+        <xdr:cNvPr id="18" name="Picture 17" descr="11979070_aogwrkdu-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -759,7 +804,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="11978892_drrprdwm-m.jpg"/>
+        <xdr:cNvPr id="19" name="Picture 18" descr="11979041_bvddbsaq-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -797,7 +842,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="11978888_gorpcrpy-m.jpg"/>
+        <xdr:cNvPr id="20" name="Picture 19" descr="11979033_xbolvyqm-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -835,7 +880,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20" descr="11978882_mcnbabpz-m.jpg"/>
+        <xdr:cNvPr id="21" name="Picture 20" descr="11979029_jxiajtun-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -873,7 +918,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21" descr="11978860_jjvducvg-m.jpg"/>
+        <xdr:cNvPr id="22" name="Picture 21" descr="11979023_nxxmpqll-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -911,7 +956,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22" descr="11978854_mkmjzwwi-m.jpg"/>
+        <xdr:cNvPr id="23" name="Picture 22" descr="11979019_ppejxyhj-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -949,7 +994,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23" descr="11978844_nbdmfmub-m.jpg"/>
+        <xdr:cNvPr id="24" name="Picture 23" descr="11979016_bbckowbn-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -987,7 +1032,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24" descr="11978836_ldatdrob-m.jpg"/>
+        <xdr:cNvPr id="25" name="Picture 24" descr="11979010_bnwglwfx-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1025,7 +1070,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25" descr="11978825_uwofoxau-m.jpg"/>
+        <xdr:cNvPr id="26" name="Picture 25" descr="11979004_xitfbetj-m.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1039,6 +1084,3350 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3429000" y="60998100"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26" descr="11978901_vxrfzpph-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="63531750"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27" descr="11978900_yqmzthau-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="66065400"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28" descr="11978892_drrprdwm-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="68599050"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="11978888_gorpcrpy-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="71132700"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="11978882_mcnbabpz-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="73666350"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31" descr="11978860_jjvducvg-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="76200000"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="11978854_mkmjzwwi-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="78733650"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33" descr="11978844_nbdmfmub-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="81267300"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34" descr="11978836_ldatdrob-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="83800950"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35" descr="11978825_uwofoxau-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="86334600"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36" descr="11978811_ydkacqqc-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="88868250"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37" descr="11978804_fxyudnoj-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="91401900"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38" descr="11978793_kyhyajjm-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="93935550"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39" descr="11978784_gnwhhhxo-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="96469200"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40" descr="11978781_ywigibbo-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="99002850"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41" descr="11978775_rmuqwsaf-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="101536500"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42" descr="11978770_jnzchymr-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="104070150"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43" descr="11978763_pebzdnov-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="106603800"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44" descr="11976085_naluarjf-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="109137450"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45" descr="11976083_qdrbdruj-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="111671100"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46" descr="11976074_cryooabx-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="114204750"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47" descr="11976072_vqzdsbbx-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="116738400"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48" descr="11976063_eftgpohl-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="119272050"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49" descr="11976060_besohmmu-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="121805700"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50" descr="11976057_cwofiprt-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="124339350"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51" descr="11976054_hqlwhizi-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="126873000"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52" descr="11976050_jnryinea-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="129406650"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53" descr="11976048_psehcgwj-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="131940300"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54" descr="11976047_zimadjob-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="134473950"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55" descr="11976042_xnzotdur-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="137007600"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56" descr="11976039_nbwljlzg-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="139541250"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57" descr="11976036_etschklr-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="142074900"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58" descr="11976033_jlnulyba-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="144608550"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59" descr="11976023_awmczoqc-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="147142200"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60" descr="11976004_daarhlbq-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="149675850"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61" descr="11976001_zxykybfq-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="152209500"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 62" descr="11975993_mippejai-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="154743150"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63" descr="11971852_tircmcfm-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="157276800"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 64" descr="11971836_akbkygtv-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="159810450"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 65" descr="11971827_hxczvqdx-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="162344100"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 66" descr="11971816_tinnyqmh-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="164877750"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Picture 67" descr="11971805_jovpxyst-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="167411400"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Picture 68" descr="11971790_ulxgqkry-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="169945050"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Picture 69" descr="11971729_zhhpqsxj-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="172478700"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Picture 70" descr="11971704_vtrhfhvd-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId70"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="175012350"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 71" descr="11971683_zlbwjlov-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId71"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="177546000"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 72" descr="11971651_aadvfkbx-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId72"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="180079650"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73" descr="11971613_daaqoggv-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId73"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="182613300"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74" descr="11971592_abcqijsi-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId74"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="185146950"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75" descr="11970628_irnfoycz-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId75"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="187680600"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Picture 76" descr="11970601_tmxbjqdd-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId76"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="190214250"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Picture 77" descr="11970592_zyywdmiw-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId77"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="192747900"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="79" name="Picture 78" descr="11970585_mtgdvuxw-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId78"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="195281550"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="80" name="Picture 79" descr="11970571_ytkggarj-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId79"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="197815200"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Picture 80" descr="11966020_nbufudpw-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId80"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="200348850"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Picture 81" descr="11965844_qbeomove-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId81"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="202882500"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="Picture 82" descr="11965827_yawaimcp-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId82"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="205416150"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="Picture 83" descr="11965813_mpnjylhj-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId83"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="207949800"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="85" name="Picture 84" descr="11965790_hdzwdgjr-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId84"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="210483450"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="86" name="Picture 85" descr="11965780_pieutwwi-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId85"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="213017100"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="87" name="Picture 86" descr="11965761_lmrhbqep-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId86"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="215550750"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="88" name="Picture 87" descr="11965738_apblzuuy-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId87"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="218084400"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="89" name="Picture 88" descr="11965715_qfkodprs-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId88"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="220618050"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="90" name="Picture 89" descr="11965695_plfwkyuu-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId89"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="223151700"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="91" name="Picture 90" descr="11965682_nciytlng-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId90"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="225685350"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="92" name="Picture 91" descr="11965661_jloueoja-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId91"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="228219000"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="93" name="Picture 92" descr="11965571_lzrunxko-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId92"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="230752650"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="94" name="Picture 93" descr="11965556_fyrmcbno-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId93"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="233286300"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="95" name="Picture 94" descr="11965540_inugkxph-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId94"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="235819950"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="96" name="Picture 95" descr="11965519_dcwvndef-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId95"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="238353600"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="97" name="Picture 96" descr="11965501_gmleuvjz-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId96"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="240887250"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="98" name="Picture 97" descr="11965466_qsmmzjqr-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId97"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="243420900"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="99" name="Picture 98" descr="11965454_hifegjfb-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId98"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="245954550"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="100" name="Picture 99" descr="11965428_lxuxsvto-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId99"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="248488200"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="101" name="Picture 100" descr="11965409_exirxhoo-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId100"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="251021850"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="102" name="Picture 101" descr="11965390_hrnaqzhq-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId101"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="253555500"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="103" name="Picture 102" descr="11965375_spdfvhha-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId102"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="256089150"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="104" name="Picture 103" descr="11964091_mreztvdy-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId103"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="258622800"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="105" name="Picture 104" descr="11962751_cbpjifzd-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId104"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="261156450"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="106" name="Picture 105" descr="11962716_fuhbgqdy-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId105"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="263690100"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="107" name="Picture 106" descr="11961689_tswnxymx-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId106"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="266223750"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="108" name="Picture 107" descr="11961678_xxatmsce-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId107"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="268757400"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="109" name="Picture 108" descr="11961016_qqmccefp-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId108"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="271291050"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="110" name="Picture 109" descr="11962413_urzjhdkt-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId109"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="273824700"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="111" name="Picture 110" descr="11962369_ibvhzahp-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId110"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="276358350"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="112" name="Picture 111" descr="11962339_ojuyjisi-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId111"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="278892000"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="113" name="Picture 112" descr="11962315_qvmhkeuh-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId112"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="281425650"/>
+          <a:ext cx="2540000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="114" name="Picture 113" descr="11961461_qdrskmcz-m.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId113"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3429000" y="283959300"/>
           <a:ext cx="2540000" cy="2540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1336,7 +4725,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1372,7 +4761,16 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>11979107</v>
+        <v>11979172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="200" customHeight="1">
@@ -1380,7 +4778,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>11979104</v>
+        <v>11979168</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="200" customHeight="1">
@@ -1388,16 +4786,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>11979097</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
+        <v>11979165</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="200" customHeight="1">
@@ -1405,7 +4794,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>11979093</v>
+        <v>11979159</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="200" customHeight="1">
@@ -1413,7 +4802,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>11979084</v>
+        <v>11979157</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="200" customHeight="1">
@@ -1421,7 +4810,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>11979075</v>
+        <v>11979153</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="200" customHeight="1">
@@ -1429,31 +4818,31 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>11979070</v>
+        <v>11979146</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="200" customHeight="1">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>11979041</v>
+        <v>11979140</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="200" customHeight="1">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>11979033</v>
+        <v>11979139</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="200" customHeight="1">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>11979029</v>
+        <v>11979129</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="200" customHeight="1">
@@ -1461,7 +4850,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>11979023</v>
+        <v>11979107</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="200" customHeight="1">
@@ -1469,7 +4858,7 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>11979019</v>
+        <v>11979104</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="200" customHeight="1">
@@ -1477,7 +4866,16 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>11979016</v>
+        <v>11979097</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="200" customHeight="1">
@@ -1485,7 +4883,7 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>11979010</v>
+        <v>11979093</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="200" customHeight="1">
@@ -1493,7 +4891,7 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <v>11979004</v>
+        <v>11979084</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="200" customHeight="1">
@@ -1501,7 +4899,7 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>11978901</v>
+        <v>11979075</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="200" customHeight="1">
@@ -1509,75 +4907,779 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <v>11978900</v>
+        <v>11979070</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="200" customHeight="1">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>11978892</v>
+        <v>11979041</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="200" customHeight="1">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B20">
-        <v>11978888</v>
+        <v>11979033</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="200" customHeight="1">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B21">
-        <v>11978882</v>
+        <v>11979029</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="200" customHeight="1">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>11978860</v>
+        <v>11979023</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="200" customHeight="1">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B23">
-        <v>11978854</v>
+        <v>11979019</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="200" customHeight="1">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B24">
-        <v>11978844</v>
+        <v>11979016</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="200" customHeight="1">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B25">
-        <v>11978836</v>
+        <v>11979010</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="200" customHeight="1">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B26">
+        <v>11979004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="200" customHeight="1">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>11978901</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="200" customHeight="1">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>11978900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="200" customHeight="1">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>11978892</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="200" customHeight="1">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>11978888</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="200" customHeight="1">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31">
+        <v>11978882</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="200" customHeight="1">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>11978860</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="200" customHeight="1">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33">
+        <v>11978854</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="200" customHeight="1">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34">
+        <v>11978844</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="200" customHeight="1">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <v>11978836</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="200" customHeight="1">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
         <v>11978825</v>
       </c>
     </row>
+    <row r="37" spans="1:2" ht="200" customHeight="1">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>11978811</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="200" customHeight="1">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>11978804</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="200" customHeight="1">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>11978793</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="200" customHeight="1">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>11978784</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="200" customHeight="1">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>11978781</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="200" customHeight="1">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>11978775</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="200" customHeight="1">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>11978770</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="200" customHeight="1">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44">
+        <v>11978763</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="200" customHeight="1">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>11976085</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="200" customHeight="1">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>11976083</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="200" customHeight="1">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>11976074</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="200" customHeight="1">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>11976072</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="200" customHeight="1">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49">
+        <v>11976063</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="200" customHeight="1">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50">
+        <v>11976060</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="200" customHeight="1">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51">
+        <v>11976057</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="200" customHeight="1">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>11976054</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="200" customHeight="1">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53">
+        <v>11976050</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="200" customHeight="1">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54">
+        <v>11976048</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="200" customHeight="1">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55">
+        <v>11976047</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="200" customHeight="1">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56">
+        <v>11976042</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="200" customHeight="1">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57">
+        <v>11976039</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="200" customHeight="1">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58">
+        <v>11976036</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="200" customHeight="1">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59">
+        <v>11976033</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="200" customHeight="1">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60">
+        <v>11976023</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="200" customHeight="1">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61">
+        <v>11976004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="200" customHeight="1">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62">
+        <v>11976001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="200" customHeight="1">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63">
+        <v>11975993</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="200" customHeight="1">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64">
+        <v>11971852</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="200" customHeight="1">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65">
+        <v>11971836</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="200" customHeight="1">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66">
+        <v>11971827</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="200" customHeight="1">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67">
+        <v>11971816</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="200" customHeight="1">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68">
+        <v>11971805</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="200" customHeight="1">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69">
+        <v>11971790</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="200" customHeight="1">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70">
+        <v>11971729</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="200" customHeight="1">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71">
+        <v>11971704</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="200" customHeight="1">
+      <c r="A72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72">
+        <v>11971683</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="200" customHeight="1">
+      <c r="A73" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73">
+        <v>11971651</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="200" customHeight="1">
+      <c r="A74" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74">
+        <v>11971613</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="200" customHeight="1">
+      <c r="A75" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75">
+        <v>11971592</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="200" customHeight="1">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76">
+        <v>11970628</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="200" customHeight="1">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77">
+        <v>11970601</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="200" customHeight="1">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78">
+        <v>11970592</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="200" customHeight="1">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79">
+        <v>11970585</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="200" customHeight="1">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80">
+        <v>11970571</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="200" customHeight="1">
+      <c r="A81" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81">
+        <v>11966020</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="200" customHeight="1">
+      <c r="A82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82">
+        <v>11965844</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="200" customHeight="1">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83">
+        <v>11965827</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="200" customHeight="1">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84">
+        <v>11965813</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="200" customHeight="1">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85">
+        <v>11965790</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="200" customHeight="1">
+      <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86">
+        <v>11965780</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="200" customHeight="1">
+      <c r="A87" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87">
+        <v>11965761</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="200" customHeight="1">
+      <c r="A88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88">
+        <v>11965738</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="200" customHeight="1">
+      <c r="A89" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89">
+        <v>11965715</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="200" customHeight="1">
+      <c r="A90" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90">
+        <v>11965695</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="200" customHeight="1">
+      <c r="A91" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91">
+        <v>11965682</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="200" customHeight="1">
+      <c r="A92" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92">
+        <v>11965661</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="200" customHeight="1">
+      <c r="A93" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93">
+        <v>11965571</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="200" customHeight="1">
+      <c r="A94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94">
+        <v>11965556</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="200" customHeight="1">
+      <c r="A95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95">
+        <v>11965540</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="200" customHeight="1">
+      <c r="A96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96">
+        <v>11965519</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="200" customHeight="1">
+      <c r="A97" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97">
+        <v>11965501</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="200" customHeight="1">
+      <c r="A98" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98">
+        <v>11965466</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="200" customHeight="1">
+      <c r="A99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99">
+        <v>11965454</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="200" customHeight="1">
+      <c r="A100" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100">
+        <v>11965428</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="200" customHeight="1">
+      <c r="A101" t="s">
+        <v>21</v>
+      </c>
+      <c r="B101">
+        <v>11965409</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="200" customHeight="1">
+      <c r="A102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102">
+        <v>11965390</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="200" customHeight="1">
+      <c r="A103" t="s">
+        <v>21</v>
+      </c>
+      <c r="B103">
+        <v>11965375</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="200" customHeight="1">
+      <c r="A104" t="s">
+        <v>22</v>
+      </c>
+      <c r="B104">
+        <v>11964091</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="200" customHeight="1">
+      <c r="A105" t="s">
+        <v>23</v>
+      </c>
+      <c r="B105">
+        <v>11962751</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="200" customHeight="1">
+      <c r="A106" t="s">
+        <v>23</v>
+      </c>
+      <c r="B106">
+        <v>11962716</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="200" customHeight="1">
+      <c r="A107" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107">
+        <v>11961689</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="200" customHeight="1">
+      <c r="A108" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108">
+        <v>11961678</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="200" customHeight="1">
+      <c r="A109" t="s">
+        <v>23</v>
+      </c>
+      <c r="B109">
+        <v>11961016</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="200" customHeight="1">
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110">
+        <v>11962413</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="200" customHeight="1">
+      <c r="A111" t="s">
+        <v>24</v>
+      </c>
+      <c r="B111">
+        <v>11962369</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="200" customHeight="1">
+      <c r="A112" t="s">
+        <v>24</v>
+      </c>
+      <c r="B112">
+        <v>11962339</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="200" customHeight="1">
+      <c r="A113" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113">
+        <v>11962315</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="200" customHeight="1">
+      <c r="A114" t="s">
+        <v>25</v>
+      </c>
+      <c r="B114">
+        <v>11961461</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F26"/>
+  <autoFilter ref="A1:F114"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Cache images for write to configuration.xlsx
</commit_message>
<xml_diff>
--- a/downloader/configuration.xlsx
+++ b/downloader/configuration.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$185</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Nazev</t>
   </si>
@@ -42,25 +42,16 @@
     <t>Vedlejsi barvy</t>
   </si>
   <si>
-    <t>Hrneček presso</t>
-  </si>
-  <si>
-    <t>typ1</t>
-  </si>
-  <si>
-    <t>style1</t>
-  </si>
-  <si>
-    <t>othercolor1</t>
-  </si>
-  <si>
-    <t>typ2</t>
-  </si>
-  <si>
-    <t>style2</t>
-  </si>
-  <si>
-    <t>othercolor2</t>
+    <t>Hrneček piccolo</t>
+  </si>
+  <si>
+    <t>mrizka</t>
+  </si>
+  <si>
+    <t>st1</t>
+  </si>
+  <si>
+    <t>col2</t>
   </si>
 </sst>
 </file>
@@ -126,13 +117,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:colOff>1905000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="11980474_hzdewbnx-m.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="11980685.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -146,7 +137,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3429000" y="190500"/>
-          <a:ext cx="2540000" cy="2540000"/>
+          <a:ext cx="1905000" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -164,13 +155,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:colOff>1905000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="11980466_vatwcxbk-m.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="11980678.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -183,8 +174,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3429000" y="2724150"/>
-          <a:ext cx="2540000" cy="2540000"/>
+          <a:off x="3429000" y="2095500"/>
+          <a:ext cx="1905000" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -483,18 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="6" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="6" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -517,12 +507,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>11980474</v>
+        <v>11980685</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -534,25 +524,198 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>11980466</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
+        <v>11980678</v>
       </c>
     </row>
+    <row r="4" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="150" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:F3"/>
+  <autoFilter ref="A1:F185"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>